<commit_message>
Broke down first Alt. More to do
</commit_message>
<xml_diff>
--- a/CH-153 Custom Grouping.xlsx
+++ b/CH-153 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A032221D-ABCB-4E92-ADFA-7A7D16CD45FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F334FEF4-9782-48FD-B632-A9722592022F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +112,14 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +162,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -335,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -407,6 +419,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,7 +1152,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="488" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1465,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AB3065-D588-4473-9F4F-1425B193655B}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,26 +1494,27 @@
     <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26"/>
       <c r="E1"/>
-      <c r="G1" s="27" t="s">
+      <c r="H1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="J1" s="6" t="s">
+      <c r="I1" s="28"/>
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
@@ -1505,14 +1523,14 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2"/>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14">
         <v>45292</v>
       </c>
@@ -1520,19 +1538,25 @@
         <v>45312</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3"/>
-      <c r="G3" s="14">
+      <c r="E3" s="29">
         <v>45292</v>
       </c>
-      <c r="H3" s="16">
+      <c r="F3" s="29">
+        <v>45312</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="14">
+        <v>45292</v>
+      </c>
+      <c r="I3" s="16">
         <v>45316</v>
       </c>
-      <c r="I3" s="9"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="9"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11">
         <v>45309</v>
       </c>
@@ -1540,19 +1564,25 @@
         <v>45316</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4"/>
-      <c r="G4" s="10">
+      <c r="E4" s="29">
+        <v>45309</v>
+      </c>
+      <c r="F4" s="29">
+        <v>45316</v>
+      </c>
+      <c r="G4" s="29"/>
+      <c r="H4" s="10">
         <v>45318</v>
       </c>
-      <c r="H4" s="17">
+      <c r="I4" s="17">
         <v>45361</v>
       </c>
-      <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="9"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10">
         <v>45318</v>
       </c>
@@ -1560,19 +1590,25 @@
         <v>45356</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5"/>
-      <c r="G5" s="18">
+      <c r="E5" s="29">
+        <v>45318</v>
+      </c>
+      <c r="F5" s="29">
+        <v>45356</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="18">
         <v>45390</v>
       </c>
-      <c r="H5" s="20">
+      <c r="I5" s="20">
         <v>45403</v>
       </c>
-      <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="9"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10">
         <v>45349</v>
       </c>
@@ -1580,19 +1616,25 @@
         <v>45352</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6"/>
-      <c r="G6" s="23">
+      <c r="E6" s="29">
+        <v>45349</v>
+      </c>
+      <c r="F6" s="29">
+        <v>45352</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="23">
         <v>45405</v>
       </c>
-      <c r="H6" s="24">
+      <c r="I6" s="24">
         <v>45408</v>
       </c>
-      <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="9"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10">
         <v>45355</v>
       </c>
@@ -1600,11 +1642,17 @@
         <v>45361</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7"/>
-      <c r="G7" s="5"/>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="29">
+        <v>45355</v>
+      </c>
+      <c r="F7" s="29">
+        <v>45361</v>
+      </c>
+      <c r="G7" s="29"/>
+      <c r="H7" s="5"/>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10">
         <v>45357</v>
       </c>
@@ -1612,16 +1660,21 @@
         <v>45359</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8"/>
-      <c r="G8" s="5"/>
-      <c r="H8"/>
+      <c r="E8" s="29">
+        <v>45357</v>
+      </c>
+      <c r="F8" s="29">
+        <v>45359</v>
+      </c>
+      <c r="G8" s="29"/>
+      <c r="H8" s="5"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
-    </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
         <v>45390</v>
       </c>
@@ -1629,16 +1682,21 @@
         <v>45392</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9"/>
-      <c r="G9" s="5"/>
-      <c r="H9"/>
+      <c r="E9" s="29">
+        <v>45390</v>
+      </c>
+      <c r="F9" s="29">
+        <v>45392</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="5"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
-    </row>
-    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18">
         <v>45391</v>
       </c>
@@ -1646,16 +1704,21 @@
         <v>45403</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10"/>
-      <c r="G10" s="5"/>
-      <c r="H10"/>
+      <c r="E10" s="29">
+        <v>45391</v>
+      </c>
+      <c r="F10" s="29">
+        <v>45403</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10" s="5"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
-    </row>
-    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="21">
         <v>45405</v>
       </c>
@@ -1663,34 +1726,40 @@
         <v>45408</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11"/>
-      <c r="G11" s="5"/>
-      <c r="H11"/>
+      <c r="E11" s="29">
+        <v>45405</v>
+      </c>
+      <c r="F11" s="29">
+        <v>45408</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="5"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11"/>
-    </row>
-    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8"/>
       <c r="F12"/>
-      <c r="G12" s="5"/>
-      <c r="H12"/>
+      <c r="G12"/>
+      <c r="H12" s="5"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" s="14" cm="1">
         <f t="array" aca="1" ref="B14:C17" ca="1">0 +
     _xlfn.TEXTSPLIT(
@@ -1720,9 +1789,33 @@
         <v>45316</v>
       </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E14" s="8" t="str" cm="1">
+        <f t="array" aca="1" ref="E14:E22" ca="1">_xlfn.SCAN(
+                        "00001|00001",
+                        C3:C11,
+                        _xlfn.LAMBDA(_xlpm.a,_xlpm.x,
+                            _xlfn.LET(
+                                _xlpm.d, _xlfn.XLOOKUP(_xlpm.x, B3:B11, C3:C11, , -1),
+                                IF(_xlpm.d &gt; 0 + RIGHT(_xlpm.a, 5), OFFSET(_xlpm.x, , -1) &amp; "|" &amp; _xlpm.d, _xlpm.a)
+                            )
+                        )
+                    )</f>
+        <v>45292|45316</v>
+      </c>
+      <c r="G14" t="str" cm="1">
+        <f t="array" aca="1" ref="G14:G17" ca="1">"|"&amp;_xlfn.UNIQUE(_xlfn.ANCHORARRAY(E14))</f>
+        <v>|45292|45316</v>
+      </c>
+      <c r="H14" s="5" t="str" cm="1">
+        <f t="array" aca="1" ref="H14:I17" ca="1">_xlfn.TEXTSPLIT(_xlfn.TEXTAFTER(_xlfn.ANCHORARRAY(G14),"|",{1,2}),"|")</f>
+        <v>45292</v>
+      </c>
+      <c r="I14" t="str">
+        <f ca="1"/>
+        <v>45316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="10">
         <f ca="1"/>
@@ -1733,9 +1826,24 @@
         <v>45361</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E15" s="8" t="str">
+        <f ca="1"/>
+        <v>45292|45316</v>
+      </c>
+      <c r="G15" t="str">
+        <f ca="1"/>
+        <v>|45318|45361</v>
+      </c>
+      <c r="H15" s="5" t="str">
+        <f ca="1"/>
+        <v>45318</v>
+      </c>
+      <c r="I15" t="str">
+        <f ca="1"/>
+        <v>45361</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="18">
         <f ca="1"/>
@@ -1746,9 +1854,24 @@
         <v>45403</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E16" s="8" t="str">
+        <f ca="1"/>
+        <v>45318|45361</v>
+      </c>
+      <c r="G16" t="str">
+        <f ca="1"/>
+        <v>|45390|45403</v>
+      </c>
+      <c r="H16" s="5" t="str">
+        <f ca="1"/>
+        <v>45390</v>
+      </c>
+      <c r="I16" t="str">
+        <f ca="1"/>
+        <v>45403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="23">
         <f ca="1"/>
@@ -1759,54 +1882,188 @@
         <v>45408</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E17" s="8" t="str">
+        <f ca="1"/>
+        <v>45318|45361</v>
+      </c>
+      <c r="G17" t="str">
+        <f ca="1"/>
+        <v>|45405|45408</v>
+      </c>
+      <c r="H17" s="5" t="str">
+        <f ca="1"/>
+        <v>45405</v>
+      </c>
+      <c r="I17" t="str">
+        <f ca="1"/>
+        <v>45408</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E18" s="8" t="str">
+        <f ca="1"/>
+        <v>45318|45361</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
+      <c r="B19" s="30">
+        <v>45292</v>
+      </c>
+      <c r="C19" s="31">
+        <v>45316</v>
+      </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E19" s="8" t="str">
+        <f ca="1"/>
+        <v>45318|45361</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
+      <c r="B20" s="30">
+        <v>45318</v>
+      </c>
+      <c r="C20" s="31">
+        <v>45361</v>
+      </c>
       <c r="D20" s="7"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="str">
+        <f ca="1"/>
+        <v>45390|45403</v>
+      </c>
+      <c r="G20" t="str" cm="1">
+        <f t="array" aca="1" ref="G20:G23" ca="1">_xlfn.UNIQUE(_xlfn.ANCHORARRAY(E14))</f>
+        <v>45292|45316</v>
+      </c>
+      <c r="H20" s="5" cm="1">
+        <f t="array" aca="1" ref="H20:I23" ca="1">_xlfn.DROP(_xlfn.REDUCE("",_xlfn.ANCHORARRAY(G20),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1)+0</f>
+        <v>45292</v>
+      </c>
+      <c r="I20">
+        <f ca="1"/>
+        <v>45316</v>
+      </c>
+      <c r="K20" t="b" cm="1">
+        <f t="array" aca="1" ref="K20:L23" ca="1">_xlfn.ANCHORARRAY(H20)=_xlfn.ANCHORARRAY(B14)</f>
+        <v>1</v>
+      </c>
+      <c r="L20" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
+      <c r="B21" s="30">
+        <v>45390</v>
+      </c>
+      <c r="C21" s="31">
+        <v>45403</v>
+      </c>
       <c r="D21" s="7"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="str">
+        <f ca="1"/>
+        <v>45390|45403</v>
+      </c>
+      <c r="G21" t="str">
+        <f ca="1"/>
+        <v>45318|45361</v>
+      </c>
+      <c r="H21" s="5">
+        <f ca="1"/>
+        <v>45318</v>
+      </c>
+      <c r="I21">
+        <f ca="1"/>
+        <v>45361</v>
+      </c>
+      <c r="K21" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="L21" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
+      <c r="B22" s="30">
+        <v>45405</v>
+      </c>
+      <c r="C22" s="31">
+        <v>45408</v>
+      </c>
       <c r="D22" s="7"/>
-      <c r="E22" s="1"/>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="str">
+        <f ca="1"/>
+        <v>45405|45408</v>
+      </c>
+      <c r="G22" t="str">
+        <f ca="1"/>
+        <v>45390|45403</v>
+      </c>
+      <c r="H22" s="5">
+        <f ca="1"/>
+        <v>45390</v>
+      </c>
+      <c r="I22">
+        <f ca="1"/>
+        <v>45403</v>
+      </c>
+      <c r="K22" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="L22" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="D23" s="7"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G23" t="str">
+        <f ca="1"/>
+        <v>45405|45408</v>
+      </c>
+      <c r="H23" s="5">
+        <f ca="1"/>
+        <v>45405</v>
+      </c>
+      <c r="I23">
+        <f ca="1"/>
+        <v>45408</v>
+      </c>
+      <c r="K23" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="L23" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D24" s="7"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D25" s="7"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D26" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Text description of the algorithm
</commit_message>
<xml_diff>
--- a/CH-153 Custom Grouping.xlsx
+++ b/CH-153 Custom Grouping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C6808C-B93D-4EF9-AA83-7BCD42848A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E110BB3-15E5-4FCD-ADB3-9D26F5140724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,6 +407,11 @@
     <xf numFmtId="14" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -419,11 +424,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,6 +910,193 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>158262</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>52754</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>29308</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38C9E2B5-03BA-1D7E-3DF5-C445BA971A2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7121770" y="515816"/>
+          <a:ext cx="4185138" cy="1975338"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>I want to describe the algorithm. There is a</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> lot of good stuff here.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1000" kern="1200" baseline="0">
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="274320" indent="-457200">
+            <a:tabLst>
+              <a:tab pos="274320" algn="l"/>
+              <a:tab pos="548640" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>•	Grab each item in "to" (call x) list</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="274320" indent="-457200">
+            <a:tabLst>
+              <a:tab pos="274320" algn="l"/>
+              <a:tab pos="548640" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>•	Look for item in "from"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> list just small or equal to "to" item</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="274320" indent="-457200">
+            <a:tabLst>
+              <a:tab pos="274320" algn="l"/>
+              <a:tab pos="548640" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>•	if the "to" item corresponding to the "from"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> item is larger than x, replace x.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="274320" indent="-457200">
+            <a:tabLst>
+              <a:tab pos="274320" algn="l"/>
+              <a:tab pos="548640" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>•	iterate through all items to ensure</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> I have found them all.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="274320" indent="-457200">
+            <a:tabLst>
+              <a:tab pos="274320" algn="l"/>
+              <a:tab pos="548640" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1000" kern="1200" baseline="0">
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0">
+            <a:tabLst>
+              <a:tab pos="274320" algn="l"/>
+              <a:tab pos="548640" algn="l"/>
+            </a:tabLst>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The accumular is interesting in that it contains two pieces of information.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1168,6 +1355,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1197,15 +1387,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="29"/>
       <c r="E1"/>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="31"/>
       <c r="J1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1484,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AB3065-D588-4473-9F4F-1425B193655B}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1501,15 +1691,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="29"/>
       <c r="E1"/>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="28"/>
+      <c r="I1" s="31"/>
       <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1538,13 +1728,13 @@
         <v>45312</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="29">
+      <c r="E3" s="25">
         <v>45292</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="25">
         <v>45312</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="14">
         <v>45292</v>
       </c>
@@ -1564,13 +1754,13 @@
         <v>45316</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="29">
+      <c r="E4" s="25">
         <v>45309</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="25">
         <v>45316</v>
       </c>
-      <c r="G4" s="29"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="10">
         <v>45318</v>
       </c>
@@ -1590,13 +1780,13 @@
         <v>45356</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="29">
+      <c r="E5" s="25">
         <v>45318</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="25">
         <v>45356</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="18">
         <v>45390</v>
       </c>
@@ -1616,13 +1806,13 @@
         <v>45352</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="29">
+      <c r="E6" s="25">
         <v>45349</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="25">
         <v>45352</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="23">
         <v>45405</v>
       </c>
@@ -1642,13 +1832,13 @@
         <v>45361</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="29">
+      <c r="E7" s="25">
         <v>45355</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="25">
         <v>45361</v>
       </c>
-      <c r="G7" s="29"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="5"/>
       <c r="I7"/>
     </row>
@@ -1660,13 +1850,13 @@
         <v>45359</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="29">
+      <c r="E8" s="25">
         <v>45357</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="25">
         <v>45359</v>
       </c>
-      <c r="G8" s="29"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="5"/>
       <c r="I8"/>
       <c r="J8"/>
@@ -1682,13 +1872,13 @@
         <v>45392</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="29">
+      <c r="E9" s="25">
         <v>45390</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="25">
         <v>45392</v>
       </c>
-      <c r="G9" s="29"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="5"/>
       <c r="I9"/>
       <c r="J9"/>
@@ -1704,13 +1894,13 @@
         <v>45403</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="29">
+      <c r="E10" s="25">
         <v>45391</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="25">
         <v>45403</v>
       </c>
-      <c r="G10" s="29"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="5"/>
       <c r="I10"/>
       <c r="J10"/>
@@ -1726,13 +1916,13 @@
         <v>45408</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="29">
+      <c r="E11" s="25">
         <v>45405</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="25">
         <v>45408</v>
       </c>
-      <c r="G11" s="29"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="5"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -1909,10 +2099,10 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="30">
+      <c r="B19" s="26">
         <v>45292</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="27">
         <v>45316</v>
       </c>
       <c r="D19" s="7"/>
@@ -1923,10 +2113,10 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="30">
+      <c r="B20" s="26">
         <v>45318</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="27">
         <v>45361</v>
       </c>
       <c r="D20" s="7"/>
@@ -1957,10 +2147,10 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="30">
+      <c r="B21" s="26">
         <v>45390</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="27">
         <v>45403</v>
       </c>
       <c r="D21" s="7"/>
@@ -1991,10 +2181,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="30">
+      <c r="B22" s="26">
         <v>45405</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="27">
         <v>45408</v>
       </c>
       <c r="D22" s="7"/>

</xml_diff>

<commit_message>
I made my first start at a model
</commit_message>
<xml_diff>
--- a/CH-153 Custom Grouping.xlsx
+++ b/CH-153 Custom Grouping.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E110BB3-15E5-4FCD-ADB3-9D26F5140724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907E6805-C97C-4E34-BEEC-71716B02C526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
+    <sheet name="EDA" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_F">EDA!$B$3:$B$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$2:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">EDA!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$26</definedName>
+    <definedName name="_T">EDA!$C$3:$C$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="5">
   <si>
     <t>Question</t>
   </si>
@@ -347,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -423,6 +427,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1090,8 +1097,81 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The accumular is interesting in that it contains two pieces of information.</a:t>
+            <a:t>The accumulator is interesting in that it contains two pieces of information.</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>670869</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>327913</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Arrow: Right 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02CC85A4-F128-4534-B051-DAC6FC826AD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1570029" y="2110740"/>
+          <a:ext cx="327604" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1339,7 +1419,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="488" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="791" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1672,10 +1752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AB3065-D588-4473-9F4F-1425B193655B}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2253,45 +2333,114 @@
         <f t="array" ref="E26:E34">_xlfn.XLOOKUP(C3:C11,B3:B11,C3:C11,,-1)</f>
         <v>45316</v>
       </c>
+      <c r="H26" s="5" t="str" cm="1">
+        <f t="array" aca="1" ref="H26:H38" ca="1">_xlfn.SCAN(
+                        "00001|00001",
+                        C5:C17,
+                        _xlfn.LAMBDA(_xlpm.a,_xlpm.x,
+                            _xlfn.LET(
+                                _xlpm.d, _xlfn.XLOOKUP(_xlpm.x, B3:B11, C3:C11, , -1),
+                                IF(_xlpm.d &gt; 0 + RIGHT(_xlpm.a, 5), OFFSET(_xlpm.x, , -1) &amp; "|" &amp; _xlpm.d, _xlpm.a)
+                            )
+                        )
+                    )</f>
+        <v>45318|45361</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E27">
         <v>45316</v>
       </c>
+      <c r="H27" s="5" t="str">
+        <f ca="1"/>
+        <v>45318|45361</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E28">
         <v>45361</v>
       </c>
+      <c r="H28" s="5" t="str">
+        <f ca="1"/>
+        <v>45318|45361</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E29">
         <v>45352</v>
       </c>
+      <c r="H29" s="5" t="str">
+        <f ca="1"/>
+        <v>45318|45361</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E30">
         <v>45359</v>
       </c>
+      <c r="H30" s="5" t="str">
+        <f ca="1"/>
+        <v>45390|45403</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E31">
         <v>45359</v>
       </c>
+      <c r="H31" s="5" t="str">
+        <f ca="1"/>
+        <v>45390|45403</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E32">
         <v>45403</v>
       </c>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="H32" s="5" t="str">
+        <f ca="1"/>
+        <v>45405|45408</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E33">
         <v>45403</v>
       </c>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="H33" s="5" t="str">
+        <f ca="1"/>
+        <v>45405|45408</v>
+      </c>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E34">
         <v>45408</v>
+      </c>
+      <c r="H34" s="5" t="str">
+        <f ca="1"/>
+        <v>45405|45408</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="5" t="str">
+        <f ca="1"/>
+        <v>45405|45408</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="5" t="str">
+        <f ca="1"/>
+        <v>45405|45408</v>
+      </c>
+    </row>
+    <row r="37" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="H37" s="5" t="str">
+        <f ca="1"/>
+        <v>45405|45408</v>
+      </c>
+    </row>
+    <row r="38" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="H38" s="5" t="str">
+        <f ca="1"/>
+        <v>45405|45408</v>
       </c>
     </row>
   </sheetData>
@@ -2303,4 +2452,356 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A17DC3C-AC30-4EFD-A813-F6B9270CAC10}">
+  <dimension ref="A1:M26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="E1"/>
+      <c r="G1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="31"/>
+      <c r="J1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2"/>
+      <c r="G2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="14">
+        <v>45292</v>
+      </c>
+      <c r="C3" s="15">
+        <v>45312</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3"/>
+      <c r="G3" s="14">
+        <v>45292</v>
+      </c>
+      <c r="H3" s="16">
+        <v>45316</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11">
+        <v>45309</v>
+      </c>
+      <c r="C4" s="16">
+        <v>45316</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4"/>
+      <c r="G4" s="10">
+        <v>45318</v>
+      </c>
+      <c r="H4" s="17">
+        <v>45361</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="10">
+        <v>45318</v>
+      </c>
+      <c r="C5" s="17">
+        <v>45356</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5"/>
+      <c r="G5" s="18">
+        <v>45390</v>
+      </c>
+      <c r="H5" s="20">
+        <v>45403</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="10">
+        <v>45349</v>
+      </c>
+      <c r="C6" s="17">
+        <v>45352</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6"/>
+      <c r="G6" s="23">
+        <v>45405</v>
+      </c>
+      <c r="H6" s="24">
+        <v>45408</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="10">
+        <v>45355</v>
+      </c>
+      <c r="C7" s="17">
+        <v>45361</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7"/>
+      <c r="G7" s="5"/>
+      <c r="H7"/>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="10">
+        <v>45357</v>
+      </c>
+      <c r="C8" s="17">
+        <v>45359</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8"/>
+      <c r="G8" s="5"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18">
+        <v>45390</v>
+      </c>
+      <c r="C9" s="19">
+        <v>45392</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9"/>
+      <c r="G9" s="5"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="18">
+        <v>45391</v>
+      </c>
+      <c r="C10" s="20">
+        <v>45403</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10"/>
+      <c r="G10" s="5"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21">
+        <v>45405</v>
+      </c>
+      <c r="C11" s="22">
+        <v>45408</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11"/>
+      <c r="G11" s="5"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+      <c r="C12"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12"/>
+      <c r="G12" s="5"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D13" s="7"/>
+      <c r="E13" s="18">
+        <v>45390</v>
+      </c>
+      <c r="F13" s="32" t="str" cm="1">
+        <f t="array" aca="1" ref="F13:F21" ca="1">_xlfn.LAMBDA(_xlpm.f,
+    _xlfn.LET(
+        _xlpm.t, _xlfn.XLOOKUP(_xlpm.f,_F,_T),
+        _xlfn.SCAN(
+            _xlpm.f&amp;"|"&amp;_xlpm.t,
+            _T,
+            _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.LET(_xlpm.d, _xlfn.XLOOKUP(_xlpm.v, B3:B11, C3:C11, , -1), IF(AND(_xlpm.d &gt; 0 + RIGHT(_xlpm.a, 5),OFFSET(_xlpm.v,,-1)=_xlpm.f), OFFSET(_xlpm.v, , -1) &amp; "|" &amp; _xlpm.d, _xlpm.a)
+                           )
+                  )
+            )
+        )
+        )(E13)</f>
+        <v>45390|45392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" t="str">
+        <f ca="1"/>
+        <v>45390|45392</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" t="str">
+        <f ca="1"/>
+        <v>45390|45392</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" t="str">
+        <f ca="1"/>
+        <v>45390|45392</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" t="str">
+        <f ca="1"/>
+        <v>45390|45392</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" t="str">
+        <f ca="1"/>
+        <v>45390|45392</v>
+      </c>
+      <c r="J18" t="str">
+        <f>TEXT(45403,"dd-mm-yyyy")</f>
+        <v>21-04-2024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" t="str">
+        <f ca="1"/>
+        <v>45390|45403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="1"/>
+      <c r="F20" t="str">
+        <f ca="1"/>
+        <v>45390|45403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="1"/>
+      <c r="F21" t="str">
+        <f ca="1"/>
+        <v>45390|45403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="1"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D24" s="7"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D25" s="7"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D26" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I couldn't leave it alone. Did an execution trace.
</commit_message>
<xml_diff>
--- a/CH-153 Custom Grouping.xlsx
+++ b/CH-153 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740435A3-7948-4FCE-80A8-4E8738D80A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A183F2-97B0-4A93-9FEF-0C9279B43981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,7 +123,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +172,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -351,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,6 +443,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1754,8 +1769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47AB3065-D588-4473-9F4F-1425B193655B}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1809,10 +1824,10 @@
         <v>45312</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="25">
+      <c r="E3" s="33">
         <v>45292</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="34">
         <v>45312</v>
       </c>
       <c r="G3" s="25"/>
@@ -1913,7 +1928,7 @@
         <v>45361</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="25">
+      <c r="E7" s="35">
         <v>45355</v>
       </c>
       <c r="F7" s="25">

</xml_diff>

<commit_message>
Continuing to try to understand this algorithm
</commit_message>
<xml_diff>
--- a/CH-153 Custom Grouping.xlsx
+++ b/CH-153 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A183F2-97B0-4A93-9FEF-0C9279B43981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE060AC-E6DD-446C-93D4-11C792FD4F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1770,7 +1770,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Trying different date combinations
</commit_message>
<xml_diff>
--- a/CH-153 Custom Grouping.xlsx
+++ b/CH-153 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE060AC-E6DD-446C-93D4-11C792FD4F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CF82EA-2BFB-43A2-B937-60BA2565CBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,6 +431,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -443,9 +446,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1482,15 +1482,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
+      <c r="C1" s="33"/>
       <c r="E1"/>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="32"/>
+      <c r="H1" s="35"/>
       <c r="J1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1770,7 +1770,7 @@
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1787,15 +1787,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
+      <c r="C1" s="33"/>
       <c r="E1"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="32"/>
+      <c r="I1" s="35"/>
       <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1824,10 +1824,11 @@
         <v>45312</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="33">
+      <c r="E3" s="29" cm="1">
+        <f t="array" ref="E3:F10">B3:C10</f>
         <v>45292</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="30">
         <v>45312</v>
       </c>
       <c r="G3" s="25"/>
@@ -1870,14 +1871,14 @@
     </row>
     <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10">
-        <v>45318</v>
+        <v>45311</v>
       </c>
       <c r="C5" s="17">
         <v>45356</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="25">
-        <v>45318</v>
+        <v>45311</v>
       </c>
       <c r="F5" s="25">
         <v>45356</v>
@@ -1928,7 +1929,7 @@
         <v>45361</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="35">
+      <c r="E7" s="31">
         <v>45355</v>
       </c>
       <c r="F7" s="25">
@@ -2012,9 +2013,7 @@
         <v>45408</v>
       </c>
       <c r="D11" s="7"/>
-      <c r="E11" s="25">
-        <v>45405</v>
-      </c>
+      <c r="E11" s="25"/>
       <c r="F11" s="25">
         <v>45408</v>
       </c>
@@ -2072,7 +2071,7 @@
       </c>
       <c r="C14" s="16">
         <f ca="1"/>
-        <v>45316</v>
+        <v>45356</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="str" cm="1">
@@ -2086,11 +2085,11 @@
                             )
                         )
                     )</f>
-        <v>45292|45316</v>
+        <v>45292|45356</v>
       </c>
       <c r="G14" t="str" cm="1">
         <f t="array" aca="1" ref="G14:G17" ca="1">"|"&amp;_xlfn.UNIQUE(_xlfn.ANCHORARRAY(E14))</f>
-        <v>|45292|45316</v>
+        <v>|45292|45356</v>
       </c>
       <c r="H14" s="5" t="str" cm="1">
         <f t="array" aca="1" ref="H14:I17" ca="1">_xlfn.TEXTSPLIT(_xlfn.TEXTAFTER(_xlfn.ANCHORARRAY(G14),"|",{1,2}),"|")</f>
@@ -2098,14 +2097,14 @@
       </c>
       <c r="I14" t="str">
         <f ca="1"/>
-        <v>45316</v>
+        <v>45356</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="10">
         <f ca="1"/>
-        <v>45318</v>
+        <v>45311</v>
       </c>
       <c r="C15" s="17">
         <f ca="1"/>
@@ -2114,15 +2113,15 @@
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="str">
         <f ca="1"/>
-        <v>45292|45316</v>
+        <v>45292|45356</v>
       </c>
       <c r="G15" t="str">
         <f ca="1"/>
-        <v>|45318|45361</v>
+        <v>|45311|45361</v>
       </c>
       <c r="H15" s="5" t="str">
         <f ca="1"/>
-        <v>45318</v>
+        <v>45311</v>
       </c>
       <c r="I15" t="str">
         <f ca="1"/>
@@ -2142,7 +2141,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="str">
         <f ca="1"/>
-        <v>45318|45361</v>
+        <v>45311|45361</v>
       </c>
       <c r="G16" t="str">
         <f ca="1"/>
@@ -2170,7 +2169,7 @@
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="str">
         <f ca="1"/>
-        <v>45318|45361</v>
+        <v>45311|45361</v>
       </c>
       <c r="G17" t="str">
         <f ca="1"/>
@@ -2190,7 +2189,7 @@
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="str">
         <f ca="1"/>
-        <v>45318|45361</v>
+        <v>45311|45361</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -2204,7 +2203,7 @@
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="str">
         <f ca="1"/>
-        <v>45318|45361</v>
+        <v>45311|45361</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -2222,7 +2221,7 @@
       </c>
       <c r="G20" t="str" cm="1">
         <f t="array" aca="1" ref="G20:G23" ca="1">_xlfn.UNIQUE(_xlfn.ANCHORARRAY(E14))</f>
-        <v>45292|45316</v>
+        <v>45292|45356</v>
       </c>
       <c r="H20" s="5" cm="1">
         <f t="array" aca="1" ref="H20:I23" ca="1">_xlfn.DROP(_xlfn.REDUCE("",_xlfn.ANCHORARRAY(G20),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.TEXTSPLIT(_xlpm.v,"|")))),1)+0</f>
@@ -2230,7 +2229,7 @@
       </c>
       <c r="I20">
         <f ca="1"/>
-        <v>45316</v>
+        <v>45356</v>
       </c>
       <c r="K20" t="b" cm="1">
         <f t="array" aca="1" ref="K20:L23" ca="1">_xlfn.ANCHORARRAY(H20)=_xlfn.ANCHORARRAY(B14)</f>
@@ -2256,11 +2255,11 @@
       </c>
       <c r="G21" t="str">
         <f ca="1"/>
-        <v>45318|45361</v>
+        <v>45311|45361</v>
       </c>
       <c r="H21" s="5">
         <f ca="1"/>
-        <v>45318</v>
+        <v>45311</v>
       </c>
       <c r="I21">
         <f ca="1"/>
@@ -2351,7 +2350,7 @@
       <c r="D26" s="7"/>
       <c r="E26" cm="1">
         <f t="array" ref="E26:E34">_xlfn.XLOOKUP(C3:C11,B3:B11,C3:C11,,-1)</f>
-        <v>45316</v>
+        <v>45356</v>
       </c>
       <c r="G26" s="1">
         <f>_xlfn.XLOOKUP(C6,B3:B11,C3:C11,,-1)</f>
@@ -2368,7 +2367,7 @@
                             )
                         )
                     )</f>
-        <v>45292|45316</v>
+        <v>45292|45356</v>
       </c>
       <c r="I26" s="1" cm="1">
         <f t="array" aca="1" ref="I26:J26" ca="1">_xlfn.TEXTSPLIT(H26,"|")+0</f>
@@ -2376,12 +2375,12 @@
       </c>
       <c r="J26" s="1">
         <f ca="1"/>
-        <v>45316</v>
+        <v>45356</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E27">
-        <v>45316</v>
+        <v>45356</v>
       </c>
       <c r="G27" s="1">
         <f>_xlfn.XLOOKUP(C7,B3:B11,C3:C11,,-1)</f>
@@ -2389,7 +2388,7 @@
       </c>
       <c r="H27" s="5" t="str">
         <f ca="1"/>
-        <v>45292|45316</v>
+        <v>45292|45356</v>
       </c>
       <c r="I27" s="1" cm="1">
         <f t="array" aca="1" ref="I27:J27" ca="1">_xlfn.TEXTSPLIT(H27,"|")+0</f>
@@ -2397,7 +2396,7 @@
       </c>
       <c r="J27" s="1">
         <f ca="1"/>
-        <v>45316</v>
+        <v>45356</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -2406,11 +2405,11 @@
       </c>
       <c r="H28" s="5" t="str">
         <f ca="1"/>
-        <v>45318|45361</v>
+        <v>45311|45361</v>
       </c>
       <c r="I28" s="1" cm="1">
         <f t="array" aca="1" ref="I28:J28" ca="1">_xlfn.TEXTSPLIT(H28,"|")+0</f>
-        <v>45318</v>
+        <v>45311</v>
       </c>
       <c r="J28" s="1">
         <f ca="1"/>
@@ -2423,11 +2422,11 @@
       </c>
       <c r="H29" s="5" t="str">
         <f ca="1"/>
-        <v>45318|45361</v>
+        <v>45311|45361</v>
       </c>
       <c r="I29" s="1" cm="1">
         <f t="array" aca="1" ref="I29:J29" ca="1">_xlfn.TEXTSPLIT(H29,"|")+0</f>
-        <v>45318</v>
+        <v>45311</v>
       </c>
       <c r="J29" s="1">
         <f ca="1"/>
@@ -2440,11 +2439,11 @@
       </c>
       <c r="H30" s="5" t="str">
         <f ca="1"/>
-        <v>45318|45361</v>
+        <v>45311|45361</v>
       </c>
       <c r="I30" s="1" cm="1">
         <f t="array" aca="1" ref="I30:J30" ca="1">_xlfn.TEXTSPLIT(H30,"|")+0</f>
-        <v>45318</v>
+        <v>45311</v>
       </c>
       <c r="J30" s="1">
         <f ca="1"/>
@@ -2457,11 +2456,11 @@
       </c>
       <c r="H31" s="5" t="str">
         <f ca="1"/>
-        <v>45318|45361</v>
+        <v>45311|45361</v>
       </c>
       <c r="I31" s="1" cm="1">
         <f t="array" aca="1" ref="I31:J31" ca="1">_xlfn.TEXTSPLIT(H31,"|")+0</f>
-        <v>45318</v>
+        <v>45311</v>
       </c>
       <c r="J31" s="1">
         <f ca="1"/>
@@ -2562,7 +2561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A17DC3C-AC30-4EFD-A813-F6B9270CAC10}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -2579,15 +2578,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
+      <c r="C1" s="33"/>
       <c r="E1"/>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="32"/>
+      <c r="H1" s="35"/>
       <c r="J1" s="6" t="s">
         <v>4</v>
       </c>

</xml_diff>